<commit_message>
Updates to component specs and euler angles documents
</commit_message>
<xml_diff>
--- a/COMPONENTS/ComponentSpecs.xlsx
+++ b/COMPONENTS/ComponentSpecs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renkert2\Documents\ARG_Research\QuadrotorOptimization\COMPONENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7E528E-DDCC-41B9-AF8F-06A6AAC03184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48C791A-DD64-45B0-8ADD-A1FEC712D3CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-3600" windowWidth="16440" windowHeight="28440" xr2:uid="{9A7CFA26-54F4-489F-A7E4-77AB580373C8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Item</t>
   </si>
@@ -51,9 +51,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>Quadrotor</t>
   </si>
   <si>
     <t>500mm Frame Kit</t>
@@ -153,7 +150,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,14 +168,6 @@
     <font>
       <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -218,7 +207,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -238,15 +227,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="thick">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -256,36 +236,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="3" xfId="4" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="3" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="5">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Total" xfId="4" builtinId="25"/>
+    <cellStyle name="Total" xfId="3" builtinId="25"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -597,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4ED600-AE82-4212-9207-193C80B590DF}">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:G7"/>
+      <selection sqref="A1:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,11 +584,11 @@
     <col min="3" max="3" width="34.42578125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -630,286 +604,268 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2" s="7">
+        <f>E2*F2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3"/>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="G3" s="11">
-        <f>E3*F3</f>
-        <v>0</v>
-      </c>
-      <c r="H3" s="4"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="5"/>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="11">
+      <c r="F3" s="7">
         <f>0.51855-(0.026*4)</f>
         <v>0.41454999999999997</v>
       </c>
-      <c r="G4" s="11">
-        <f t="shared" ref="G4:G14" si="0">E4*F4</f>
+      <c r="G3" s="7">
+        <f>E3*F3</f>
         <v>0.41454999999999997</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4">
+        <v>4</v>
+      </c>
+      <c r="F4" s="7">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="G4" s="7">
+        <f>E4*F4</f>
+        <v>0.104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="11">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="G5" s="11">
-        <f>F5*4</f>
-        <v>0.104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="5"/>
+      <c r="F5" s="7">
+        <f>0.2624/4</f>
+        <v>6.5600000000000006E-2</v>
+      </c>
+      <c r="G5" s="7">
+        <f t="shared" ref="G5:G13" si="0">E5*F5</f>
+        <v>0.26240000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>4</v>
       </c>
-      <c r="F6" s="11">
-        <f>0.2624/4</f>
-        <v>6.5600000000000006E-2</v>
-      </c>
-      <c r="G6" s="11">
-        <f t="shared" si="0"/>
-        <v>0.26240000000000002</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7">
-        <v>4</v>
-      </c>
-      <c r="F7" s="11">
+      <c r="F6" s="7">
         <f>0.0491/4</f>
         <v>1.2274999999999999E-2</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G6" s="7">
         <f t="shared" si="0"/>
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="11" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="11">
+      <c r="F8" s="7">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G9" s="11">
+      <c r="G8" s="7">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>21</v>
       </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" s="11">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
         <v>5.9450000000000003E-2</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G9" s="7">
         <f t="shared" si="0"/>
         <v>5.9450000000000003E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="G11" s="11">
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="G10" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12" s="11">
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" s="7">
         <v>1.9050000000000001E-2</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G11" s="7">
         <f t="shared" si="0"/>
         <v>1.9050000000000001E-2</v>
       </c>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
         <v>27</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D12" t="s">
         <v>28</v>
       </c>
-      <c r="D13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="11">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12" s="7">
         <v>0.47735</v>
       </c>
-      <c r="G13" s="11">
+      <c r="G12" s="7">
         <f t="shared" si="0"/>
         <v>0.47735</v>
       </c>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
         <v>30</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D13" t="s">
         <v>31</v>
       </c>
-      <c r="D14" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" s="11">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" s="7">
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G13" s="7">
         <f t="shared" si="0"/>
         <v>1.5699999999999999E-2</v>
       </c>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
+    </row>
+    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12">
-        <f>SUM(G3:G14)</f>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8">
+        <f>SUM(G2:G13)</f>
         <v>1.4716</v>
       </c>
-      <c r="H15" s="8"/>
-    </row>
-    <row r="16" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>33</v>
+    </row>
+    <row r="15" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A3" r:id="rId1" xr:uid="{DAA3B178-F289-4BBF-A66B-B91DD34069F2}"/>
-    <hyperlink ref="A12" r:id="rId2" xr:uid="{9E604536-B6CB-4815-880C-F81049848033}"/>
-    <hyperlink ref="A13" r:id="rId3" xr:uid="{4964F84B-92D2-40C7-AB2D-CEBC0B3609BE}"/>
-    <hyperlink ref="A14" r:id="rId4" xr:uid="{45F879AA-2543-4E6A-A3DB-04B61E06E7C2}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{DAA3B178-F289-4BBF-A66B-B91DD34069F2}"/>
+    <hyperlink ref="A11" r:id="rId2" xr:uid="{9E604536-B6CB-4815-880C-F81049848033}"/>
+    <hyperlink ref="A12" r:id="rId3" xr:uid="{4964F84B-92D2-40C7-AB2D-CEBC0B3609BE}"/>
+    <hyperlink ref="A13" r:id="rId4" xr:uid="{45F879AA-2543-4E6A-A3DB-04B61E06E7C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>

</xml_diff>

<commit_message>
Removed CAD Files from Repo
</commit_message>
<xml_diff>
--- a/COMPONENTS/ComponentSpecs.xlsx
+++ b/COMPONENTS/ComponentSpecs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renkert2\Documents\ARG_Research\QuadrotorOptimization\COMPONENTS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prenk\Box\ARG_Research\QuadrotorOptimization\COMPONENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48C791A-DD64-45B0-8ADD-A1FEC712D3CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C907D050-4143-4B90-94C5-64A8384FEE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3600" windowWidth="16440" windowHeight="28440" xr2:uid="{9A7CFA26-54F4-489F-A7E4-77AB580373C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9A7CFA26-54F4-489F-A7E4-77AB580373C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -574,21 +574,21 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G16"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="1" max="1" width="22.109375" customWidth="1"/>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+    <col min="3" max="3" width="34.44140625" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -611,7 +611,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -626,7 +626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" t="s">
         <v>8</v>
@@ -646,7 +646,7 @@
         <v>0.41454999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" t="s">
         <v>10</v>
@@ -665,7 +665,7 @@
         <v>0.104</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" t="s">
         <v>12</v>
@@ -685,7 +685,7 @@
         <v>0.26240000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" t="s">
         <v>14</v>
@@ -705,7 +705,7 @@
         <v>4.9099999999999998E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" t="s">
         <v>16</v>
@@ -723,7 +723,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" t="s">
         <v>18</v>
@@ -742,7 +742,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" t="s">
         <v>20</v>
@@ -761,7 +761,7 @@
         <v>5.9450000000000003E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="3"/>
       <c r="B10" t="s">
         <v>22</v>
@@ -777,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>24</v>
       </c>
@@ -798,7 +798,7 @@
         <v>1.9050000000000001E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
@@ -819,7 +819,7 @@
         <v>0.47735</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>29</v>
       </c>
@@ -840,7 +840,7 @@
         <v>1.5699999999999999E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
@@ -854,8 +854,8 @@
         <v>1.4716</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>32</v>
       </c>

</xml_diff>

<commit_message>
Added inertia matrix estimate to Quadrotor
</commit_message>
<xml_diff>
--- a/COMPONENTS/ComponentSpecs.xlsx
+++ b/COMPONENTS/ComponentSpecs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prenk\Box\ARG_Research\QuadrotorOptimization\COMPONENTS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C907D050-4143-4B90-94C5-64A8384FEE7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F207C7-5930-42C4-B0C5-46FC67B46CF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9A7CFA26-54F4-489F-A7E4-77AB580373C8}"/>
   </bookViews>
@@ -574,7 +574,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>